<commit_message>
some benchmark tests, and simpler models for R matrix
</commit_message>
<xml_diff>
--- a/benchmark/algo_evaluation.xlsx
+++ b/benchmark/algo_evaluation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\3A\Stage3A\code longitudinal models\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861BBF04-4B86-4FF6-8C34-BACB3C6ABF0C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74AE294-F881-4B43-9EB6-F7F6D7A23F8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="56">
   <si>
     <t>dataset</t>
   </si>
@@ -84,9 +84,6 @@
     <t>true</t>
   </si>
   <si>
-    <t>visual inspection: pred. Σ = gt Σ ?</t>
-  </si>
-  <si>
     <t>source of ground truth (gt)</t>
   </si>
   <si>
@@ -138,34 +135,97 @@
     <t>no</t>
   </si>
   <si>
-    <t>didn't compute gt Σ, but 'no' for R</t>
-  </si>
-  <si>
     <t>[1.546, 2.412]</t>
   </si>
   <si>
     <t>[0.343,  -0.515]</t>
   </si>
   <si>
-    <t>[0.501, 0.358]</t>
-  </si>
-  <si>
     <t>playground_data/benchmark2</t>
   </si>
   <si>
-    <t>no* (+ gt threw warning)</t>
-  </si>
-  <si>
-    <t>*: lavann w.r.t. the returned variances: "[...] they are dependent (or endogenous) variables (predicted by the latent variables), and therefore, the value for the variance that is printed in the output is an estimate of the residual variance: the left-over variance that is not explained by the predictor(s)."</t>
+    <t>BFGS (3-point) (uncorrelated errors)</t>
+  </si>
+  <si>
+    <r>
+      <t>lavaan (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>no</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> covariance struct)</t>
+    </r>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>visual inspection: pred. R = gt R ?</t>
+  </si>
+  <si>
+    <t>[76.419, -4.082, 1.170]</t>
+  </si>
+  <si>
+    <t>[-0.089, -0.117, 0.044]</t>
+  </si>
+  <si>
+    <t>[76.4188771, -4.08157274, 1.17016249]</t>
+  </si>
+  <si>
+    <t>[-0.0894226522, -0.116600821, 0.0438990616]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.501, 0.358] </t>
+  </si>
+  <si>
+    <t>[1.55114224, 2.36334553]</t>
+  </si>
+  <si>
+    <t>[0.32880025,             -0.36559861]</t>
+  </si>
+  <si>
+    <t>[0.50650685, 0.29611999]</t>
+  </si>
+  <si>
+    <t>gt threw warning</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>yes ('negative variances')</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>no convergence even w/o covariance in R; lavaan preds were the same !</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -184,7 +244,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,8 +263,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -221,16 +287,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -250,17 +359,120 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -536,385 +748,749 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.21875" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="2" max="2" width="13" style="6" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
-    <col min="6" max="6" width="7.88671875" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" style="7" customWidth="1"/>
-    <col min="8" max="9" width="7.44140625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="6.33203125" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" style="7" customWidth="1"/>
-    <col min="12" max="12" width="14.21875" style="7" customWidth="1"/>
-    <col min="15" max="15" width="27.77734375" customWidth="1"/>
-    <col min="16" max="16" width="27.109375" customWidth="1"/>
+    <col min="4" max="4" width="23.109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" customWidth="1"/>
+    <col min="7" max="7" width="7.88671875" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="7.21875" style="6" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="6.33203125" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" style="6" customWidth="1"/>
+    <col min="13" max="13" width="14.21875" style="6" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" customWidth="1"/>
+    <col min="16" max="16" width="14.77734375" style="6" customWidth="1"/>
+    <col min="17" max="17" width="15.33203125" style="6" customWidth="1"/>
+    <col min="18" max="18" width="17.88671875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:18" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>27</v>
+      <c r="P1" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" s="33" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>1</v>
       </c>
-      <c r="G2" s="6">
+      <c r="H2" s="5">
         <v>75.174999999999997</v>
       </c>
-      <c r="H2" s="8">
+      <c r="I2" s="7">
         <v>-0.115</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="9">
+      <c r="J2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="8">
         <v>75.175312439999999</v>
       </c>
-      <c r="L2" s="9">
+      <c r="M2" s="8">
         <v>-0.11459639000000001</v>
       </c>
-      <c r="M2" t="s">
-        <v>14</v>
-      </c>
       <c r="N2" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="O2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="R2" s="34"/>
     </row>
-    <row r="3" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="5">
+        <v>75.427000000000007</v>
+      </c>
+      <c r="I3" s="7">
+        <v>-0.114</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="28">
+        <v>75.427467550000003</v>
+      </c>
+      <c r="M3" s="8">
+        <v>-0.11442417000000001</v>
+      </c>
+      <c r="N3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="R3" s="34"/>
+    </row>
+    <row r="4" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G4" s="22">
         <v>3</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="H4" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="J4" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="N4" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q4" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="R4" s="34"/>
+    </row>
+    <row r="5" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="2">
+        <v>3</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q5" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="R5" s="35"/>
+    </row>
+    <row r="6" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" t="s">
-        <v>14</v>
-      </c>
-      <c r="N3" t="s">
-        <v>14</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="B6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="1">
+        <v>2</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R6" s="34"/>
     </row>
-    <row r="4" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="7" spans="1:18" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C7" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D7" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="22">
+        <v>2</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="N7" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="O7" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="P7" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q7" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="R7" s="34"/>
+    </row>
+    <row r="8" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="22">
+        <v>2</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="1">
+      <c r="I8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="O8" s="32"/>
+      <c r="P8" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="R8" s="34"/>
+    </row>
+    <row r="9" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="2">
         <v>2</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="7" t="s">
+      <c r="H9" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="M9" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="O9" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="P9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="R9" s="36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="7" t="s">
+      <c r="E10" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="7">
+        <v>0.89171098999999998</v>
+      </c>
+      <c r="I10" s="7">
+        <v>0.48974328</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="6">
+        <v>0.89977585000000004</v>
+      </c>
+      <c r="M10" s="6">
+        <v>0.58902807000000001</v>
+      </c>
+      <c r="N10" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="P10" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="N4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>36</v>
-      </c>
+      <c r="Q10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R10" s="34"/>
     </row>
-    <row r="5" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="11" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="1">
-        <v>2</v>
-      </c>
-      <c r="G5" s="8" t="s">
+      <c r="E11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="I11" s="7">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="8">
+        <v>0.89977585000000004</v>
+      </c>
+      <c r="M11" s="8">
+        <v>0.58902807000000001</v>
+      </c>
+      <c r="N11" t="s">
+        <v>14</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="P11" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q11" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="R11" s="34"/>
+    </row>
+    <row r="12" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="B12" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="C12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="7">
+        <v>0.89171098999999998</v>
+      </c>
+      <c r="I12" s="7">
+        <v>0.48974328</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="6">
+        <v>0.89402256000000002</v>
+      </c>
+      <c r="M12" s="6">
+        <v>0.51830231000000004</v>
+      </c>
+      <c r="N12" t="s">
+        <v>14</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R12" s="34"/>
+    </row>
+    <row r="13" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="M5" s="9" t="s">
+      <c r="E13" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="N5" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="F13" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1</v>
+      </c>
+      <c r="H13" s="29">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="I13" s="11">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L13" s="13">
+        <v>0.89402256000000002</v>
+      </c>
+      <c r="M13" s="13">
+        <v>0.51830231000000004</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P13" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-      <c r="G6" s="7">
-        <v>0.89171098999999998</v>
-      </c>
-      <c r="H6" s="7">
-        <v>0.48974328</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6" s="7">
-        <v>0.89977585000000004</v>
-      </c>
-      <c r="L6" s="7">
-        <v>0.58902807000000001</v>
-      </c>
-      <c r="M6" t="s">
-        <v>14</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="Q13" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-      <c r="G7" s="13">
-        <v>0.9</v>
-      </c>
-      <c r="H7" s="7">
-        <v>0.58899999999999997</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="9">
-        <v>0.89977585000000004</v>
-      </c>
-      <c r="L7" s="9">
-        <v>0.58902807000000001</v>
-      </c>
-      <c r="M7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="O9" s="7" t="s">
-        <v>43</v>
-      </c>
+      <c r="R13" s="35"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",E1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
implemented time-indep error with FIML/discrepancy
</commit_message>
<xml_diff>
--- a/benchmark/algo_evaluation.xlsx
+++ b/benchmark/algo_evaluation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\3A\Stage3A\code longitudinal models\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D02185B-C9AB-4CEF-8EB6-2CB1086E83CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8CA5F6-D96F-4692-9164-B57F2F27BD91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,17 +16,26 @@
     <sheet name="GCM" sheetId="1" r:id="rId1"/>
     <sheet name="color legend" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="102">
   <si>
     <t>dataset</t>
   </si>
@@ -389,6 +398,65 @@
   <si>
     <t>[-0.0890295349, -0.113642759, 0.0571854045]</t>
   </si>
+  <si>
+    <r>
+      <t>BFGS (3-point) (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>time-indep errors + FIML</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>true (with some non definite positivity)</t>
+  </si>
+  <si>
+    <t>using FIML, we had the same output as lavaan despite the non definite pos.</t>
+  </si>
+  <si>
+    <t>[1.55114714,2.36330046]</t>
+  </si>
+  <si>
+    <t>[0.34712245,-0.55662159]</t>
+  </si>
+  <si>
+    <t>[0.49531048,0.41286192]</t>
+  </si>
+  <si>
+    <t>[1.48615392, 1.58946641]</t>
+  </si>
+  <si>
+    <t>[0.54002713, 0.55357967]</t>
+  </si>
+  <si>
+    <t>[1.01165266, 0.62394241]</t>
+  </si>
+  <si>
+    <t>[76.4423757, -4.14842821, 0.952653182]</t>
+  </si>
+  <si>
+    <t>[-0.0890297604, -0.113642612, 0.0571853271]</t>
+  </si>
+  <si>
+    <t>we got the correct results, but got some warnings that lavaan did not have</t>
+  </si>
 </sst>
 </file>
 
@@ -399,7 +467,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="#,##0.0000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,6 +477,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -535,9 +611,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -547,7 +621,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -673,15 +747,143 @@
     <xf numFmtId="3" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="25">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1036,17 +1238,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U21"/>
+  <dimension ref="A1:U27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="U26" sqref="U26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.21875" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
-    <col min="3" max="4" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
     <col min="5" max="5" width="23.109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="9.5546875" style="3" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" customWidth="1"/>
@@ -1072,7 +1275,7 @@
       <c r="B1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D1" s="11" t="s">
@@ -1137,7 +1340,7 @@
       <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D2" t="s">
@@ -1200,7 +1403,7 @@
       <c r="B3" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D3" t="s">
@@ -1263,7 +1466,7 @@
       <c r="B4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D4" t="s">
@@ -1319,93 +1522,93 @@
       </c>
       <c r="U4" s="24"/>
     </row>
-    <row r="5" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+    <row r="5" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>59</v>
+      <c r="D5" t="s">
+        <v>58</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="16">
+        <v>67</v>
+      </c>
+      <c r="F5" s="3">
         <v>108</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="17" t="s">
+      <c r="G5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="14">
-        <v>3</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="L5" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="N5" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="O5" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="P5" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q5" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="R5" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="S5" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="T5" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="U5" s="24"/>
+      <c r="J5" s="1">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2">
+        <v>75.358999999999995</v>
+      </c>
+      <c r="L5" s="4">
+        <v>-0.109</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" t="s">
+        <v>14</v>
+      </c>
+      <c r="O5" s="19">
+        <v>75.359469790000006</v>
+      </c>
+      <c r="P5" s="5">
+        <v>-0.10890764999999999</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>14</v>
+      </c>
+      <c r="R5" t="s">
+        <v>14</v>
+      </c>
+      <c r="S5" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="T5" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="U5" s="58"/>
     </row>
     <row r="6" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="17" t="s">
-        <v>58</v>
+      <c r="D6" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="F6" s="16">
         <v>108</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="6" t="s">
         <v>38</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="I6" s="17" t="s">
         <v>13</v>
@@ -1414,10 +1617,10 @@
         <v>3</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="M6" s="16" t="s">
         <v>14</v>
@@ -1425,11 +1628,11 @@
       <c r="N6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="O6" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="P6" s="18" t="s">
-        <v>43</v>
+      <c r="O6" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="P6" s="39" t="s">
+        <v>24</v>
       </c>
       <c r="Q6" s="17" t="s">
         <v>14</v>
@@ -1437,11 +1640,11 @@
       <c r="R6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="S6" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="T6" s="18" t="s">
-        <v>38</v>
+      <c r="S6" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="T6" s="36" t="s">
+        <v>34</v>
       </c>
       <c r="U6" s="24"/>
     </row>
@@ -1449,17 +1652,17 @@
       <c r="A7" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="17" t="s">
+      <c r="B7" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>58</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F7" s="16">
         <v>108</v>
@@ -1477,239 +1680,243 @@
         <v>3</v>
       </c>
       <c r="K7" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="O7" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="P7" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q7" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="R7" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="S7" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="T7" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="U7" s="24"/>
+    </row>
+    <row r="8" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="16">
+        <v>108</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="14">
+        <v>3</v>
+      </c>
+      <c r="K8" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="L7" s="15" t="s">
+      <c r="L8" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="M7" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="N7" s="56" t="s">
-        <v>14</v>
-      </c>
-      <c r="O7" s="18" t="s">
+      <c r="M8" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="O8" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="P7" s="18" t="s">
+      <c r="P8" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="Q7" s="56" t="s">
-        <v>14</v>
-      </c>
-      <c r="R7" s="56" t="s">
-        <v>14</v>
-      </c>
-      <c r="S7" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="T7" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="U7" s="24"/>
-    </row>
-    <row r="8" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="26" t="s">
+      <c r="Q8" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="R8" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="S8" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="T8" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="U8" s="24"/>
+    </row>
+    <row r="9" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="59" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="16">
+        <v>108</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="14">
+        <v>3</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="L9" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="M9" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N9" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q9" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="R9" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="S9" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="T9" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="U9" s="61" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B10" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C10" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="47" t="s">
+      <c r="D10" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E10" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="29">
+      <c r="F10" s="29">
         <v>50</v>
       </c>
-      <c r="G8" s="47" t="s">
+      <c r="G10" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="H8" s="29" t="s">
+      <c r="H10" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="28" t="s">
+      <c r="I10" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="30">
+      <c r="J10" s="30">
         <v>2</v>
       </c>
-      <c r="K8" s="31" t="s">
+      <c r="K10" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="L8" s="31" t="s">
+      <c r="L10" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="M8" s="31" t="s">
+      <c r="M10" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="N8" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="O8" s="27" t="s">
+      <c r="N10" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="P8" s="27" t="s">
+      <c r="P10" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="Q8" s="27" t="s">
+      <c r="Q10" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="R8" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="S8" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="T8" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="U8" s="32"/>
-    </row>
-    <row r="9" spans="1:21" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="16">
-        <v>50</v>
-      </c>
-      <c r="G9" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="H9" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I9" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="J9" s="14">
-        <v>2</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="N9" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="O9" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="P9" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q9" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="R9" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="S9" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="T9" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="U9" s="24"/>
-    </row>
-    <row r="10" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="7">
-        <v>50</v>
-      </c>
-      <c r="G10" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="I10" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" s="14">
-        <v>2</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="N10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="P10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="R10" s="22"/>
-      <c r="S10" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="T10" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="U10" s="24"/>
-    </row>
-    <row r="11" spans="1:21" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R10" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="S10" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="T10" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="U10" s="32"/>
+    </row>
+    <row r="11" spans="1:21" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="20" t="s">
+      <c r="B11" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="21" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="33" t="s">
         <v>59</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="F11" s="16">
         <v>50</v>
@@ -1718,7 +1925,7 @@
         <v>38</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="I11" s="20" t="s">
         <v>26</v>
@@ -1726,28 +1933,28 @@
       <c r="J11" s="14">
         <v>2</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="K11" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="L11" s="15" t="s">
+      <c r="L11" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="M11" s="15" t="s">
+      <c r="M11" s="8" t="s">
         <v>44</v>
       </c>
       <c r="N11" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="O11" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="P11" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q11" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="R11" s="21" t="s">
+      <c r="O11" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="P11" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q11" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="R11" s="22" t="s">
         <v>14</v>
       </c>
       <c r="S11" s="36" t="s">
@@ -1756,22 +1963,20 @@
       <c r="T11" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="U11" s="25" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U11" s="24"/>
+    </row>
+    <row r="12" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="33" t="s">
+      <c r="B12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="21" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>31</v>
@@ -1803,41 +2008,39 @@
       <c r="N12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="O12" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="P12" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q12" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="R12" s="34" t="s">
-        <v>14</v>
-      </c>
+      <c r="O12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R12" s="22"/>
       <c r="S12" s="22" t="s">
         <v>34</v>
       </c>
       <c r="T12" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="U12" s="35"/>
+      <c r="U12" s="24"/>
     </row>
     <row r="13" spans="1:21" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="33" t="s">
+      <c r="B13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="21" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F13" s="16">
         <v>50</v>
@@ -1855,584 +2058,1035 @@
         <v>2</v>
       </c>
       <c r="K13" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="L13" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="M13" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="N13" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="O13" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="P13" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q13" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="R13" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="S13" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="T13" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="U13" s="25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="7">
+        <v>50</v>
+      </c>
+      <c r="G14" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I14" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" s="14">
+        <v>2</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O14" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="P14" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q14" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="R14" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="S14" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="T14" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="U14" s="35"/>
+    </row>
+    <row r="15" spans="1:21" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="16">
+        <v>50</v>
+      </c>
+      <c r="G15" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="14">
+        <v>2</v>
+      </c>
+      <c r="K15" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="L13" s="15" t="s">
+      <c r="L15" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="M13" s="15" t="s">
+      <c r="M15" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="N13" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="O13" s="39" t="s">
+      <c r="N15" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="O15" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="P13" s="39" t="s">
+      <c r="P15" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="Q13" s="39" t="s">
+      <c r="Q15" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="R13" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S13" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="T13" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="U13" s="25" t="s">
+      <c r="R15" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="S15" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="T15" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="U15" s="25" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="29">
-        <v>50</v>
-      </c>
-      <c r="G14" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="H14" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="I14" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="J14" s="30">
-        <v>1</v>
-      </c>
-      <c r="K14" s="31">
-        <v>0.89171098999999998</v>
-      </c>
-      <c r="L14" s="31">
-        <v>0.48974328</v>
-      </c>
-      <c r="M14" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="N14" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="O14" s="27">
-        <v>0.89977585000000004</v>
-      </c>
-      <c r="P14" s="27">
-        <v>0.58902807000000001</v>
-      </c>
-      <c r="Q14" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="R14" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="S14" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="T14" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="U14" s="32"/>
-    </row>
-    <row r="15" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="3">
-        <v>50</v>
-      </c>
-      <c r="G15" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15" s="1">
-        <v>1</v>
-      </c>
-      <c r="K15" s="9">
-        <v>0.9</v>
-      </c>
-      <c r="L15" s="4">
-        <v>0.58899999999999997</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="N15" t="s">
-        <v>14</v>
-      </c>
-      <c r="O15" s="38">
-        <v>0.89977585000000004</v>
-      </c>
-      <c r="P15" s="38">
-        <v>0.58902807000000001</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>14</v>
-      </c>
-      <c r="R15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="S15" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="T15" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="U15" s="24"/>
-    </row>
-    <row r="16" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>18</v>
+    <row r="16" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="59" t="s">
+        <v>91</v>
       </c>
       <c r="D16" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="16">
+        <v>50</v>
+      </c>
+      <c r="G16" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" s="14">
+        <v>2</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="L16" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="M16" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="N16" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="O16" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="P16" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q16" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="R16" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="S16" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="T16" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="U16" s="24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F17" s="29">
         <v>50</v>
       </c>
-      <c r="G16" s="33" t="s">
+      <c r="G17" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="H17" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I17" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J17" s="30">
         <v>1</v>
       </c>
-      <c r="K16" s="4">
+      <c r="K17" s="31">
         <v>0.89171098999999998</v>
       </c>
-      <c r="L16" s="4">
+      <c r="L17" s="31">
         <v>0.48974328</v>
       </c>
-      <c r="M16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="N16" t="s">
-        <v>14</v>
-      </c>
-      <c r="O16" s="3">
-        <v>0.89402256000000002</v>
-      </c>
-      <c r="P16" s="3">
-        <v>0.51830231000000004</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>14</v>
-      </c>
-      <c r="R16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="S16" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="T16" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="U16" s="24"/>
-    </row>
-    <row r="17" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
+      <c r="M17" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="N17" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="O17" s="27">
+        <v>0.89977585000000004</v>
+      </c>
+      <c r="P17" s="27">
+        <v>0.58902807000000001</v>
+      </c>
+      <c r="Q17" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="R17" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="S17" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="T17" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="U17" s="32"/>
+    </row>
+    <row r="18" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="3">
+        <v>50</v>
+      </c>
+      <c r="G18" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" s="1">
+        <v>1</v>
+      </c>
+      <c r="K18" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="L18" s="4">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N18" t="s">
+        <v>14</v>
+      </c>
+      <c r="O18" s="38">
+        <v>0.89977585000000004</v>
+      </c>
+      <c r="P18" s="38">
+        <v>0.58902807000000001</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>14</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S18" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="T18" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="U18" s="24"/>
+    </row>
+    <row r="19" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="F17" s="16">
-        <v>50</v>
-      </c>
-      <c r="G17" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="H17" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I17" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="J17" s="14">
-        <v>1</v>
-      </c>
-      <c r="K17" s="46">
-        <v>0.89400000000000002</v>
-      </c>
-      <c r="L17" s="15">
-        <v>0.51800000000000002</v>
-      </c>
-      <c r="M17" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="N17" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="O17" s="18">
-        <v>0.89402256000000002</v>
-      </c>
-      <c r="P17" s="18">
-        <v>0.51830231000000004</v>
-      </c>
-      <c r="Q17" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="R17" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="S17" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="T17" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="U17" s="24"/>
-    </row>
-    <row r="18" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="21">
-        <v>50</v>
-      </c>
-      <c r="G18" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="H18" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="I18" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="J18" s="14">
-        <v>1</v>
-      </c>
-      <c r="K18" s="4">
-        <v>0.89171098999999998</v>
-      </c>
-      <c r="L18" s="4">
-        <v>0.48974328</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="N18" t="s">
-        <v>14</v>
-      </c>
-      <c r="O18" s="16">
-        <v>0.87162667000000005</v>
-      </c>
-      <c r="P18" s="16">
-        <v>0.55798082999999998</v>
-      </c>
-      <c r="Q18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="R18" t="s">
-        <v>14</v>
-      </c>
-      <c r="S18" s="16"/>
-      <c r="T18" s="16"/>
-      <c r="U18" s="24"/>
-    </row>
-    <row r="19" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D19" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="7">
+        <v>50</v>
+      </c>
+      <c r="G19" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J19" s="1">
+        <v>1</v>
+      </c>
+      <c r="K19" s="4">
+        <v>0.89171098999999998</v>
+      </c>
+      <c r="L19" s="4">
+        <v>0.48974328</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N19" t="s">
+        <v>14</v>
+      </c>
+      <c r="O19" s="3">
+        <v>0.89402256000000002</v>
+      </c>
+      <c r="P19" s="3">
+        <v>0.51830231000000004</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>14</v>
+      </c>
+      <c r="R19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="T19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="U19" s="24"/>
+    </row>
+    <row r="20" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="16">
+        <v>50</v>
+      </c>
+      <c r="G20" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I20" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J20" s="14">
+        <v>1</v>
+      </c>
+      <c r="K20" s="46">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="L20" s="15">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="M20" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N20" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="O20" s="18">
+        <v>0.89402256000000002</v>
+      </c>
+      <c r="P20" s="18">
+        <v>0.51830231000000004</v>
+      </c>
+      <c r="Q20" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="R20" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="S20" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="T20" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="U20" s="24"/>
+    </row>
+    <row r="21" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="21">
+        <v>50</v>
+      </c>
+      <c r="G21" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="I21" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J21" s="14">
+        <v>1</v>
+      </c>
+      <c r="K21" s="4">
+        <v>0.89171098999999998</v>
+      </c>
+      <c r="L21" s="4">
+        <v>0.48974328</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N21" t="s">
+        <v>14</v>
+      </c>
+      <c r="O21" s="16">
+        <v>0.87162667000000005</v>
+      </c>
+      <c r="P21" s="16">
+        <v>0.55798082999999998</v>
+      </c>
+      <c r="Q21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="R21" t="s">
+        <v>14</v>
+      </c>
+      <c r="S21" s="16"/>
+      <c r="T21" s="16"/>
+      <c r="U21" s="24"/>
+    </row>
+    <row r="22" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F19" s="16">
+      <c r="F22" s="16">
         <v>50</v>
       </c>
-      <c r="G19" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="H19" s="16" t="s">
+      <c r="G22" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="I19" s="20" t="s">
+      <c r="I22" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="J19" s="14">
+      <c r="J22" s="14">
         <v>1</v>
       </c>
-      <c r="K19" s="15">
+      <c r="K22" s="15">
         <v>0.872</v>
       </c>
-      <c r="L19" s="15">
+      <c r="L22" s="15">
         <v>0.55800000000000005</v>
       </c>
-      <c r="M19" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="N19" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="O19" s="39">
+      <c r="M22" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N22" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="O22" s="39">
         <v>0.87162667000000005</v>
       </c>
-      <c r="P19" s="39">
+      <c r="P22" s="39">
         <v>0.55798082999999998</v>
       </c>
-      <c r="Q19" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="R19" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="S19" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="T19" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="U19" s="24" t="s">
+      <c r="Q22" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="R22" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="S22" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="T22" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="U22" s="24" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="26" t="s">
+    <row r="23" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="60" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F23" s="16">
+        <v>50</v>
+      </c>
+      <c r="G23" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="I23" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J23" s="14">
+        <v>1</v>
+      </c>
+      <c r="K23" s="15">
+        <v>0.872</v>
+      </c>
+      <c r="L23" s="15">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="M23" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N23" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="O23" s="39">
+        <v>0.87162719</v>
+      </c>
+      <c r="P23" s="39">
+        <v>0.55798128000000002</v>
+      </c>
+      <c r="Q23" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="R23" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="S23" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="T23" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="U23" s="24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B24" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="47" t="s">
+      <c r="C24" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="D24" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E24" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="F20" s="27">
+      <c r="F24" s="27">
         <v>250</v>
       </c>
-      <c r="G20" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="H20" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="I20" s="26" t="s">
+      <c r="G24" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="I24" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="J20" s="30">
+      <c r="J24" s="30">
         <v>1</v>
       </c>
-      <c r="K20" s="31">
+      <c r="K24" s="31">
         <v>0.28899999999999998</v>
       </c>
-      <c r="L20" s="31">
+      <c r="L24" s="31">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="M20" s="31">
+      <c r="M24" s="31">
         <v>0.77500000000000002</v>
       </c>
-      <c r="N20" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="O20" s="48">
+      <c r="N24" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="O24" s="48">
         <v>0.28907486999999998</v>
       </c>
-      <c r="P20" s="48">
+      <c r="P24" s="48">
         <v>7.3790670000000003E-2</v>
       </c>
-      <c r="Q20" s="49">
+      <c r="Q24" s="49">
         <v>0.77539077000000001</v>
       </c>
-      <c r="R20" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="S20" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="T20" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="U20" s="55"/>
-    </row>
-    <row r="21" spans="1:21" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="26" t="s">
+      <c r="R24" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="S24" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="T24" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="U24" s="32"/>
+    </row>
+    <row r="25" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="60" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" s="16">
+        <v>250</v>
+      </c>
+      <c r="G25" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I25" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="J25" s="14">
+        <v>1</v>
+      </c>
+      <c r="K25" s="15">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="L25" s="15">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="M25" s="15">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="N25" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="O25" s="18">
+        <v>0.28907732000000003</v>
+      </c>
+      <c r="P25" s="18">
+        <v>7.3785790000000004E-2</v>
+      </c>
+      <c r="Q25" s="56">
+        <v>0.77539374999999999</v>
+      </c>
+      <c r="R25" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="S25" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="T25" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="U25" s="61" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B26" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="47" t="s">
+      <c r="C26" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="47" t="s">
+      <c r="D26" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="E21" s="27" t="s">
+      <c r="E26" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="27">
+      <c r="F26" s="27">
         <v>250</v>
       </c>
-      <c r="G21" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="H21" s="27" t="s">
+      <c r="G26" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="H26" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="I21" s="28" t="s">
+      <c r="I26" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="J21" s="30">
+      <c r="J26" s="30">
         <v>2</v>
       </c>
-      <c r="K21" s="31" t="s">
+      <c r="K26" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="L21" s="31" t="s">
+      <c r="L26" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="M21" s="31" t="s">
+      <c r="M26" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="N21" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="O21" s="50" t="s">
+      <c r="N26" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="O26" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="P21" s="50" t="s">
+      <c r="P26" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="Q21" s="54" t="s">
+      <c r="Q26" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="R21" s="51" t="s">
-        <v>14</v>
-      </c>
-      <c r="S21" s="52" t="s">
-        <v>34</v>
-      </c>
-      <c r="T21" s="52" t="s">
-        <v>34</v>
-      </c>
-      <c r="U21" s="53" t="s">
+      <c r="R26" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="S26" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="T26" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="U26" s="53" t="s">
         <v>65</v>
       </c>
     </row>
+    <row r="27" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27" s="60" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" s="16">
+        <v>250</v>
+      </c>
+      <c r="G27" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I27" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J27" s="57">
+        <v>2</v>
+      </c>
+      <c r="K27" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="L27" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="M27" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="N27" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="O27" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="P27" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q27" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="R27" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="S27" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="T27" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="U27" s="24" t="s">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="H22:H1048576 H1:H20">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+  <conditionalFormatting sqref="H27:H1048576 I25 H17:H25 H1:H4 H10:H15 H6:H8">
+    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="23" priority="24" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="yes">
+    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="yes">
       <formula>NOT(ISERROR(SEARCH("yes",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D22:D1048576 G22:G1048576 D1:D20 G1:G20">
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+  <conditionalFormatting sqref="D28:D1048576 G28:G1048576 G17:G25 G1:G4 D1:D4 G10:G15 G6:G8 D6:D25">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
       <formula>"NOT OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D22:D1048576 D1:D20">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+  <conditionalFormatting sqref="D28:D1048576 D1:D4 D6:D25">
+    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+  <conditionalFormatting sqref="H26">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",H21)))</formula>
+    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="yes">
-      <formula>NOT(ISERROR(SEARCH("yes",H21)))</formula>
+    <cfRule type="containsText" dxfId="17" priority="20" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",H26)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G21 D21">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+  <conditionalFormatting sqref="G26 D26">
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
       <formula>"NOT OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D21">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="D26">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
       <formula>"ok"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G16">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
+      <formula>"NOT OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16">
+    <cfRule type="cellIs" dxfId="13" priority="12" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="14" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",H16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G27 D27">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>"NOT OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+      <formula>"ok"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",H5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5 D5">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+      <formula>"NOT OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"ok"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",H9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G9">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"NOT OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add multistart optimization + FIML estimator w/ groups
</commit_message>
<xml_diff>
--- a/benchmark/algo_evaluation.xlsx
+++ b/benchmark/algo_evaluation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\3A\Stage3A\code longitudinal models\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8CA5F6-D96F-4692-9164-B57F2F27BD91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FB1656-AC47-4E4B-8BE7-AEFC1A02F87D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="105">
   <si>
     <t>dataset</t>
   </si>
@@ -456,6 +456,38 @@
   </si>
   <si>
     <t>we got the correct results, but got some warnings that lavaan did not have</t>
+  </si>
+  <si>
+    <r>
+      <t>BFGS (3-point) (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>uncorrelated errors + FIML</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>[76.4188733, -4.08156396, 1.17017266]</t>
+  </si>
+  <si>
+    <t>[-0.0894226178, -0.116601011, 0.0438991599]</t>
   </si>
 </sst>
 </file>
@@ -766,7 +798,124 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="40">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1238,10 +1387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U27"/>
+  <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="U26" sqref="U26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1459,26 +1608,26 @@
       </c>
       <c r="U3" s="24"/>
     </row>
-    <row r="4" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>18</v>
+        <v>102</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>91</v>
       </c>
       <c r="D4" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="16" t="s">
-        <v>67</v>
+      <c r="E4" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="F4" s="3">
         <v>108</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" t="s">
         <v>38</v>
       </c>
       <c r="H4" s="3" t="s">
@@ -1491,10 +1640,10 @@
         <v>1</v>
       </c>
       <c r="K4" s="2">
-        <v>75.358999999999995</v>
+        <v>75.427000000000007</v>
       </c>
       <c r="L4" s="4">
-        <v>-0.109</v>
+        <v>-0.114</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>14</v>
@@ -1503,10 +1652,10 @@
         <v>14</v>
       </c>
       <c r="O4" s="19">
-        <v>75.359470180000002</v>
+        <v>75.427472249999994</v>
       </c>
       <c r="P4" s="5">
-        <v>-0.10890764</v>
+        <v>-0.11442431</v>
       </c>
       <c r="Q4" t="s">
         <v>14</v>
@@ -1526,10 +1675,10 @@
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D5" t="s">
@@ -1566,10 +1715,10 @@
         <v>14</v>
       </c>
       <c r="O5" s="19">
-        <v>75.359469790000006</v>
+        <v>75.359470180000002</v>
       </c>
       <c r="P5" s="5">
-        <v>-0.10890764999999999</v>
+        <v>-0.10890764</v>
       </c>
       <c r="Q5" t="s">
         <v>14</v>
@@ -1577,101 +1726,101 @@
       <c r="R5" t="s">
         <v>14</v>
       </c>
-      <c r="S5" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="T5" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="U5" s="58"/>
+      <c r="S5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="U5" s="24"/>
     </row>
     <row r="6" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>59</v>
+        <v>90</v>
+      </c>
+      <c r="C6" s="59" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" t="s">
+        <v>58</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="16">
+        <v>67</v>
+      </c>
+      <c r="F6" s="3">
         <v>108</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="17" t="s">
+      <c r="G6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="14">
-        <v>3</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="L6" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="M6" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="N6" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="O6" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="P6" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q6" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="R6" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="S6" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="T6" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="U6" s="24"/>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2">
+        <v>75.358999999999995</v>
+      </c>
+      <c r="L6" s="4">
+        <v>-0.109</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O6" s="19">
+        <v>75.359469790000006</v>
+      </c>
+      <c r="P6" s="5">
+        <v>-0.10890764999999999</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>14</v>
+      </c>
+      <c r="R6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S6" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="T6" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="U6" s="58"/>
     </row>
     <row r="7" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="17" t="s">
-        <v>58</v>
+      <c r="D7" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="F7" s="16">
         <v>108</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="6" t="s">
         <v>38</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="I7" s="17" t="s">
         <v>13</v>
@@ -1680,10 +1829,10 @@
         <v>3</v>
       </c>
       <c r="K7" s="15" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="L7" s="15" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="M7" s="16" t="s">
         <v>14</v>
@@ -1691,11 +1840,11 @@
       <c r="N7" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="O7" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="P7" s="18" t="s">
-        <v>43</v>
+      <c r="O7" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="P7" s="39" t="s">
+        <v>24</v>
       </c>
       <c r="Q7" s="17" t="s">
         <v>14</v>
@@ -1703,11 +1852,11 @@
       <c r="R7" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="S7" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="T7" s="18" t="s">
-        <v>38</v>
+      <c r="S7" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="T7" s="36" t="s">
+        <v>34</v>
       </c>
       <c r="U7" s="24"/>
     </row>
@@ -1715,8 +1864,8 @@
       <c r="A8" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>52</v>
+      <c r="B8" s="16" t="s">
+        <v>53</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>18</v>
@@ -1725,7 +1874,7 @@
         <v>58</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F8" s="16">
         <v>108</v>
@@ -1743,27 +1892,27 @@
         <v>3</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="L8" s="15" t="s">
-        <v>87</v>
+        <v>41</v>
       </c>
       <c r="M8" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="55" t="s">
+      <c r="N8" s="17" t="s">
         <v>14</v>
       </c>
       <c r="O8" s="18" t="s">
-        <v>88</v>
+        <v>42</v>
       </c>
       <c r="P8" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q8" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="R8" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q8" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="R8" s="17" t="s">
         <v>14</v>
       </c>
       <c r="S8" s="18" t="s">
@@ -1779,16 +1928,16 @@
         <v>11</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="C9" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="D9" s="55" t="s">
+      <c r="D9" s="17" t="s">
         <v>58</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F9" s="16">
         <v>108</v>
@@ -1806,22 +1955,22 @@
         <v>3</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>87</v>
+        <v>41</v>
       </c>
       <c r="M9" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="N9" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="O9" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="P9" s="5" t="s">
-        <v>100</v>
+      <c r="N9" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="O9" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="P9" s="18" t="s">
+        <v>104</v>
       </c>
       <c r="Q9" s="55" t="s">
         <v>14</v>
@@ -1835,203 +1984,205 @@
       <c r="T9" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="U9" s="61" t="s">
-        <v>101</v>
-      </c>
+      <c r="U9" s="24"/>
     </row>
     <row r="10" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="29" t="s">
+      <c r="A10" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="47" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="29">
-        <v>50</v>
-      </c>
-      <c r="G10" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="I10" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" s="30">
-        <v>2</v>
-      </c>
-      <c r="K10" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="L10" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="M10" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="N10" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="O10" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="P10" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q10" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="R10" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="S10" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="T10" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="U10" s="32"/>
+      <c r="D10" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="16">
+        <v>108</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="14">
+        <v>3</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="L10" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="M10" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N10" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="P10" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q10" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="R10" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="S10" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="T10" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="U10" s="24"/>
     </row>
-    <row r="11" spans="1:21" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="33" t="s">
-        <v>59</v>
+        <v>90</v>
+      </c>
+      <c r="C11" s="59" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="55" t="s">
+        <v>58</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="F11" s="16">
-        <v>50</v>
-      </c>
-      <c r="G11" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="G11" s="17" t="s">
         <v>38</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I11" s="20" t="s">
-        <v>26</v>
+        <v>34</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>13</v>
       </c>
       <c r="J11" s="14">
-        <v>2</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="M11" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="N11" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="O11" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="P11" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q11" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="R11" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="S11" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="T11" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="U11" s="24"/>
+        <v>3</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="L11" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="M11" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N11" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q11" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="R11" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="S11" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="T11" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="U11" s="61" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="12" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="21" t="s">
+      <c r="B12" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="33" t="s">
+      <c r="D12" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="29">
         <v>50</v>
       </c>
-      <c r="G12" s="33" t="s">
+      <c r="G12" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="I12" s="20" t="s">
+      <c r="I12" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="14">
+      <c r="J12" s="30">
         <v>2</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="L12" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="M12" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="N12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O12" s="3" t="s">
+      <c r="N12" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="O12" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="P12" s="3" t="s">
+      <c r="P12" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="Q12" s="3" t="s">
+      <c r="Q12" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="R12" s="22"/>
-      <c r="S12" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="T12" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="U12" s="24"/>
+      <c r="R12" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="S12" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="T12" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="U12" s="32"/>
     </row>
-    <row r="13" spans="1:21" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>53</v>
+      <c r="B13" s="16" t="s">
+        <v>16</v>
       </c>
       <c r="C13" s="21" t="s">
         <v>18</v>
@@ -2040,7 +2191,7 @@
         <v>59</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="F13" s="16">
         <v>50</v>
@@ -2049,7 +2200,7 @@
         <v>38</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="I13" s="20" t="s">
         <v>26</v>
@@ -2057,28 +2208,28 @@
       <c r="J13" s="14">
         <v>2</v>
       </c>
-      <c r="K13" s="15" t="s">
+      <c r="K13" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="L13" s="15" t="s">
+      <c r="L13" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="M13" s="15" t="s">
+      <c r="M13" s="8" t="s">
         <v>44</v>
       </c>
       <c r="N13" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="O13" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="P13" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q13" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="R13" s="21" t="s">
+      <c r="O13" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="P13" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q13" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="R13" s="22" t="s">
         <v>14</v>
       </c>
       <c r="S13" s="36" t="s">
@@ -2087,22 +2238,20 @@
       <c r="T13" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="U13" s="25" t="s">
-        <v>64</v>
-      </c>
+      <c r="U13" s="24"/>
     </row>
-    <row r="14" spans="1:21" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="34" t="s">
+      <c r="B14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="21" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="33" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>31</v>
@@ -2134,41 +2283,39 @@
       <c r="N14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="O14" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="P14" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q14" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="R14" s="34" t="s">
-        <v>14</v>
-      </c>
+      <c r="O14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R14" s="22"/>
       <c r="S14" s="22" t="s">
         <v>34</v>
       </c>
       <c r="T14" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="U14" s="35"/>
+      <c r="U14" s="24"/>
     </row>
     <row r="15" spans="1:21" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="34" t="s">
+      <c r="B15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="21" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F15" s="16">
         <v>50</v>
@@ -2186,27 +2333,27 @@
         <v>2</v>
       </c>
       <c r="K15" s="15" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="L15" s="15" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="M15" s="15" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="N15" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="O15" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="P15" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q15" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="R15" s="34" t="s">
+      <c r="O15" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="P15" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q15" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="R15" s="21" t="s">
         <v>14</v>
       </c>
       <c r="S15" s="36" t="s">
@@ -2216,33 +2363,33 @@
         <v>34</v>
       </c>
       <c r="U15" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="C16" s="59" t="s">
-        <v>91</v>
+        <v>52</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>18</v>
       </c>
       <c r="D16" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16" s="16">
+      <c r="E16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="7">
         <v>50</v>
       </c>
       <c r="G16" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="I16" s="20" t="s">
         <v>26</v>
@@ -2250,321 +2397,323 @@
       <c r="J16" s="14">
         <v>2</v>
       </c>
-      <c r="K16" s="15" t="s">
+      <c r="K16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O16" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="P16" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q16" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="R16" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="S16" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="T16" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="U16" s="35"/>
+    </row>
+    <row r="17" spans="1:21" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="16">
+        <v>50</v>
+      </c>
+      <c r="G17" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" s="14">
+        <v>2</v>
+      </c>
+      <c r="K17" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="L16" s="15" t="s">
+      <c r="L17" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="M16" s="15" t="s">
+      <c r="M17" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="N16" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="O16" s="38" t="s">
+      <c r="N17" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="O17" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="P17" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q17" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="R17" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="S17" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="T17" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="U17" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="59" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="16">
+        <v>50</v>
+      </c>
+      <c r="G18" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" s="14">
+        <v>2</v>
+      </c>
+      <c r="K18" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="L18" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="M18" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="N18" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="O18" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="P16" s="38" t="s">
+      <c r="P18" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="Q16" s="38" t="s">
+      <c r="Q18" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="R16" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S16" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="T16" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="U16" s="24" t="s">
+      <c r="R18" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="S18" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="T18" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="U18" s="24" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="29">
-        <v>50</v>
-      </c>
-      <c r="G17" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="H17" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="I17" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="J17" s="30">
-        <v>1</v>
-      </c>
-      <c r="K17" s="31">
-        <v>0.89171098999999998</v>
-      </c>
-      <c r="L17" s="31">
-        <v>0.48974328</v>
-      </c>
-      <c r="M17" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="N17" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="O17" s="27">
-        <v>0.89977585000000004</v>
-      </c>
-      <c r="P17" s="27">
-        <v>0.58902807000000001</v>
-      </c>
-      <c r="Q17" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="R17" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="S17" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="T17" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="U17" s="32"/>
-    </row>
-    <row r="18" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="3">
-        <v>50</v>
-      </c>
-      <c r="G18" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J18" s="1">
-        <v>1</v>
-      </c>
-      <c r="K18" s="9">
-        <v>0.9</v>
-      </c>
-      <c r="L18" s="4">
-        <v>0.58899999999999997</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="N18" t="s">
-        <v>14</v>
-      </c>
-      <c r="O18" s="38">
-        <v>0.89977585000000004</v>
-      </c>
-      <c r="P18" s="38">
-        <v>0.58902807000000001</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>14</v>
-      </c>
-      <c r="R18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="S18" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="T18" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="U18" s="24"/>
     </row>
     <row r="19" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="7" t="s">
+      <c r="B19" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="E19" s="7" t="s">
+      <c r="D19" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="29">
         <v>50</v>
       </c>
-      <c r="G19" s="33" t="s">
+      <c r="G19" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="H19" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I19" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="J19" s="1">
+      <c r="J19" s="30">
         <v>1</v>
       </c>
-      <c r="K19" s="4">
+      <c r="K19" s="31">
         <v>0.89171098999999998</v>
       </c>
-      <c r="L19" s="4">
+      <c r="L19" s="31">
         <v>0.48974328</v>
       </c>
-      <c r="M19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="N19" t="s">
-        <v>14</v>
-      </c>
-      <c r="O19" s="3">
-        <v>0.89402256000000002</v>
-      </c>
-      <c r="P19" s="3">
-        <v>0.51830231000000004</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>14</v>
-      </c>
-      <c r="R19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="S19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="T19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="U19" s="24"/>
+      <c r="M19" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="N19" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="O19" s="27">
+        <v>0.89977585000000004</v>
+      </c>
+      <c r="P19" s="27">
+        <v>0.58902807000000001</v>
+      </c>
+      <c r="Q19" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="R19" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="S19" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="T19" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="U19" s="32"/>
     </row>
-    <row r="20" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="17" t="s">
+    <row r="20" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="21" t="s">
+      <c r="B20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D20" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="F20" s="16">
+        <v>59</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="3">
         <v>50</v>
       </c>
       <c r="G20" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="H20" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I20" s="20" t="s">
+      <c r="H20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J20" s="14">
+      <c r="J20" s="1">
         <v>1</v>
       </c>
-      <c r="K20" s="46">
-        <v>0.89400000000000002</v>
-      </c>
-      <c r="L20" s="15">
-        <v>0.51800000000000002</v>
-      </c>
-      <c r="M20" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="N20" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="O20" s="18">
-        <v>0.89402256000000002</v>
-      </c>
-      <c r="P20" s="18">
-        <v>0.51830231000000004</v>
-      </c>
-      <c r="Q20" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="R20" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="S20" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="T20" s="18" t="s">
-        <v>38</v>
+      <c r="K20" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="L20" s="4">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N20" t="s">
+        <v>14</v>
+      </c>
+      <c r="O20" s="38">
+        <v>0.89977585000000004</v>
+      </c>
+      <c r="P20" s="38">
+        <v>0.58902807000000001</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>14</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S20" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="T20" s="37" t="s">
+        <v>34</v>
       </c>
       <c r="U20" s="24"/>
     </row>
     <row r="21" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="17" t="s">
+      <c r="A21" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" s="34" t="s">
+      <c r="B21" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D21" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="E21" s="21" t="s">
+      <c r="E21" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F21" s="7">
         <v>50</v>
       </c>
       <c r="G21" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="H21" s="16" t="s">
+      <c r="H21" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="I21" s="20" t="s">
+      <c r="I21" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J21" s="14">
+      <c r="J21" s="1">
         <v>1</v>
       </c>
       <c r="K21" s="4">
@@ -2579,20 +2728,24 @@
       <c r="N21" t="s">
         <v>14</v>
       </c>
-      <c r="O21" s="16">
-        <v>0.87162667000000005</v>
-      </c>
-      <c r="P21" s="16">
-        <v>0.55798082999999998</v>
-      </c>
-      <c r="Q21" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="R21" t="s">
-        <v>14</v>
-      </c>
-      <c r="S21" s="16"/>
-      <c r="T21" s="16"/>
+      <c r="O21" s="3">
+        <v>0.89402256000000002</v>
+      </c>
+      <c r="P21" s="3">
+        <v>0.51830231000000004</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>14</v>
+      </c>
+      <c r="R21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S21" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="T21" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="U21" s="24"/>
     </row>
     <row r="22" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
@@ -2600,16 +2753,16 @@
         <v>37</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="21" t="s">
         <v>18</v>
       </c>
       <c r="D22" s="33" t="s">
         <v>58</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F22" s="16">
         <v>50</v>
@@ -2618,7 +2771,7 @@
         <v>38</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="I22" s="20" t="s">
         <v>26</v>
@@ -2626,11 +2779,11 @@
       <c r="J22" s="14">
         <v>1</v>
       </c>
-      <c r="K22" s="15">
-        <v>0.872</v>
+      <c r="K22" s="46">
+        <v>0.89400000000000002</v>
       </c>
       <c r="L22" s="15">
-        <v>0.55800000000000005</v>
+        <v>0.51800000000000002</v>
       </c>
       <c r="M22" s="16" t="s">
         <v>14</v>
@@ -2638,34 +2791,32 @@
       <c r="N22" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="O22" s="39">
-        <v>0.87162667000000005</v>
-      </c>
-      <c r="P22" s="39">
-        <v>0.55798082999999998</v>
-      </c>
-      <c r="Q22" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="R22" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="S22" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="T22" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="U22" s="24" t="s">
-        <v>74</v>
-      </c>
+      <c r="O22" s="18">
+        <v>0.89402256000000002</v>
+      </c>
+      <c r="P22" s="18">
+        <v>0.51830231000000004</v>
+      </c>
+      <c r="Q22" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="R22" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="S22" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="T22" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="U22" s="24"/>
     </row>
-    <row r="23" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="C23" s="60" t="s">
         <v>91</v>
@@ -2674,16 +2825,16 @@
         <v>58</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F23" s="16">
         <v>50</v>
       </c>
-      <c r="G23" s="34" t="s">
+      <c r="G23" s="33" t="s">
         <v>38</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="I23" s="20" t="s">
         <v>26</v>
@@ -2691,11 +2842,11 @@
       <c r="J23" s="14">
         <v>1</v>
       </c>
-      <c r="K23" s="15">
-        <v>0.872</v>
+      <c r="K23" s="46">
+        <v>0.89400000000000002</v>
       </c>
       <c r="L23" s="15">
-        <v>0.55800000000000005</v>
+        <v>0.51800000000000002</v>
       </c>
       <c r="M23" s="16" t="s">
         <v>14</v>
@@ -2703,22 +2854,22 @@
       <c r="N23" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="O23" s="39">
-        <v>0.87162719</v>
-      </c>
-      <c r="P23" s="39">
-        <v>0.55798128000000002</v>
-      </c>
-      <c r="Q23" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="R23" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="S23" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="T23" s="39" t="s">
+      <c r="O23" s="18">
+        <v>0.89402247999999995</v>
+      </c>
+      <c r="P23" s="18">
+        <v>0.51830198999999999</v>
+      </c>
+      <c r="Q23" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="R23" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="S23" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="T23" s="18" t="s">
         <v>38</v>
       </c>
       <c r="U23" s="24" t="s">
@@ -2726,367 +2877,619 @@
       </c>
     </row>
     <row r="24" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" s="27" t="s">
+      <c r="A24" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="51" t="s">
+      <c r="C24" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="26" t="s">
+      <c r="D24" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="F24" s="27">
-        <v>250</v>
-      </c>
-      <c r="G24" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="H24" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="I24" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="J24" s="30">
+      <c r="E24" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="21">
+        <v>50</v>
+      </c>
+      <c r="G24" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="I24" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J24" s="14">
         <v>1</v>
       </c>
-      <c r="K24" s="31">
-        <v>0.28899999999999998</v>
-      </c>
-      <c r="L24" s="31">
-        <v>7.3999999999999996E-2</v>
-      </c>
-      <c r="M24" s="31">
-        <v>0.77500000000000002</v>
-      </c>
-      <c r="N24" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="O24" s="48">
-        <v>0.28907486999999998</v>
-      </c>
-      <c r="P24" s="48">
-        <v>7.3790670000000003E-2</v>
-      </c>
-      <c r="Q24" s="49">
-        <v>0.77539077000000001</v>
-      </c>
-      <c r="R24" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="S24" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="T24" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="U24" s="32"/>
+      <c r="K24" s="4">
+        <v>0.89171098999999998</v>
+      </c>
+      <c r="L24" s="4">
+        <v>0.48974328</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N24" t="s">
+        <v>14</v>
+      </c>
+      <c r="O24" s="16">
+        <v>0.87162667000000005</v>
+      </c>
+      <c r="P24" s="16">
+        <v>0.55798082999999998</v>
+      </c>
+      <c r="Q24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="R24" t="s">
+        <v>14</v>
+      </c>
+      <c r="S24" s="16"/>
+      <c r="T24" s="16"/>
+      <c r="U24" s="24"/>
     </row>
-    <row r="25" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="C25" s="60" t="s">
-        <v>91</v>
-      </c>
-      <c r="D25" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="33" t="s">
         <v>58</v>
       </c>
       <c r="E25" s="16" t="s">
         <v>67</v>
       </c>
       <c r="F25" s="16">
-        <v>250</v>
-      </c>
-      <c r="G25" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="G25" s="33" t="s">
         <v>38</v>
       </c>
       <c r="H25" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I25" s="22" t="s">
-        <v>76</v>
+        <v>85</v>
+      </c>
+      <c r="I25" s="20" t="s">
+        <v>26</v>
       </c>
       <c r="J25" s="14">
         <v>1</v>
       </c>
       <c r="K25" s="15">
+        <v>0.872</v>
+      </c>
+      <c r="L25" s="15">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="M25" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N25" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="O25" s="39">
+        <v>0.87162667000000005</v>
+      </c>
+      <c r="P25" s="39">
+        <v>0.55798082999999998</v>
+      </c>
+      <c r="Q25" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="R25" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="S25" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="T25" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="U25" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="60" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="16">
+        <v>50</v>
+      </c>
+      <c r="G26" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="I26" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J26" s="14">
+        <v>1</v>
+      </c>
+      <c r="K26" s="15">
+        <v>0.872</v>
+      </c>
+      <c r="L26" s="15">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="M26" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N26" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="O26" s="39">
+        <v>0.87162719</v>
+      </c>
+      <c r="P26" s="39">
+        <v>0.55798128000000002</v>
+      </c>
+      <c r="Q26" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="R26" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="S26" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="T26" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="U26" s="24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="51" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" s="27">
+        <v>250</v>
+      </c>
+      <c r="G27" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H27" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="I27" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="J27" s="30">
+        <v>1</v>
+      </c>
+      <c r="K27" s="31">
         <v>0.28899999999999998</v>
       </c>
-      <c r="L25" s="15">
+      <c r="L27" s="31">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="M25" s="15">
+      <c r="M27" s="31">
         <v>0.77500000000000002</v>
       </c>
-      <c r="N25" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="O25" s="18">
+      <c r="N27" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="O27" s="48">
+        <v>0.28907486999999998</v>
+      </c>
+      <c r="P27" s="48">
+        <v>7.3790670000000003E-2</v>
+      </c>
+      <c r="Q27" s="49">
+        <v>0.77539077000000001</v>
+      </c>
+      <c r="R27" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="S27" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="T27" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="U27" s="32"/>
+    </row>
+    <row r="28" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="60" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" s="16">
+        <v>250</v>
+      </c>
+      <c r="G28" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I28" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="J28" s="14">
+        <v>1</v>
+      </c>
+      <c r="K28" s="15">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="L28" s="15">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="M28" s="15">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="N28" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="O28" s="18">
         <v>0.28907732000000003</v>
       </c>
-      <c r="P25" s="18">
+      <c r="P28" s="18">
         <v>7.3785790000000004E-2</v>
       </c>
-      <c r="Q25" s="56">
+      <c r="Q28" s="56">
         <v>0.77539374999999999</v>
       </c>
-      <c r="R25" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="S25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="T25" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="U25" s="61" t="s">
+      <c r="R28" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="S28" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="T28" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="U28" s="61" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="26" t="s">
+    <row r="29" spans="1:21" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B29" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="51" t="s">
+      <c r="C29" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="D26" s="47" t="s">
+      <c r="D29" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="E26" s="27" t="s">
+      <c r="E29" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="F26" s="27">
+      <c r="F29" s="27">
         <v>250</v>
       </c>
-      <c r="G26" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="H26" s="27" t="s">
+      <c r="G29" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="H29" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="I26" s="28" t="s">
+      <c r="I29" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="J26" s="30">
+      <c r="J29" s="30">
         <v>2</v>
       </c>
-      <c r="K26" s="31" t="s">
+      <c r="K29" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="L26" s="31" t="s">
+      <c r="L29" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="M26" s="31" t="s">
+      <c r="M29" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="N26" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="O26" s="50" t="s">
+      <c r="N29" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="O29" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="P26" s="50" t="s">
+      <c r="P29" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="Q26" s="54" t="s">
+      <c r="Q29" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="R26" s="51" t="s">
-        <v>14</v>
-      </c>
-      <c r="S26" s="52" t="s">
-        <v>34</v>
-      </c>
-      <c r="T26" s="52" t="s">
-        <v>34</v>
-      </c>
-      <c r="U26" s="53" t="s">
+      <c r="R29" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="S29" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="T29" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="U29" s="53" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="17" t="s">
+    <row r="30" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B30" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C27" s="60" t="s">
+      <c r="C30" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="D27" s="55" t="s">
+      <c r="D30" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E30" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F27" s="16">
+      <c r="F30" s="16">
         <v>250</v>
       </c>
-      <c r="G27" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="H27" s="3" t="s">
+      <c r="G30" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H30" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I27" s="20" t="s">
+      <c r="I30" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="J27" s="57">
+      <c r="J30" s="57">
         <v>2</v>
       </c>
-      <c r="K27" s="15" t="s">
+      <c r="K30" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="L27" s="15" t="s">
+      <c r="L30" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="M27" s="15" t="s">
+      <c r="M30" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="N27" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="O27" s="38" t="s">
+      <c r="N30" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="O30" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="P27" s="38" t="s">
+      <c r="P30" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="Q27" s="38" t="s">
+      <c r="Q30" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="R27" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="S27" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="T27" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="U27" s="24" t="s">
+      <c r="R30" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="S30" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="T30" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="U30" s="24" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H27:H1048576 I25 H17:H25 H1:H4 H10:H15 H6:H8">
-    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
+  <conditionalFormatting sqref="H30:H1048576 I28 H19:H22 H1:H3 H12:H17 H7:H8 H24:H28 H5 H10">
+    <cfRule type="cellIs" dxfId="39" priority="37" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="24" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="38" priority="39" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="yes">
+    <cfRule type="containsText" dxfId="37" priority="41" operator="containsText" text="yes">
       <formula>NOT(ISERROR(SEARCH("yes",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D28:D1048576 G28:G1048576 G17:G25 G1:G4 D1:D4 G10:G15 G6:G8 D6:D25">
-    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
+  <conditionalFormatting sqref="D31:D1048576 G31:G1048576 G19:G22 G1:G3 D1:D3 G12:G17 G7:G8 D7:D8 D24:D28 G24:G28 D5 G5 D10:D22 G10">
+    <cfRule type="cellIs" dxfId="36" priority="38" operator="equal">
       <formula>"NOT OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D28:D1048576 D1:D4 D6:D25">
-    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
+  <conditionalFormatting sqref="D31:D1048576 D1:D3 D7:D8 D24:D28 D5 D10:D22">
+    <cfRule type="cellIs" dxfId="35" priority="36" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
+  <conditionalFormatting sqref="H29">
+    <cfRule type="cellIs" dxfId="34" priority="32" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",H26)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="20" operator="containsText" text="yes">
-      <formula>NOT(ISERROR(SEARCH("yes",H26)))</formula>
+    <cfRule type="containsText" dxfId="33" priority="34" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H29)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="35" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",H29)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G26 D26">
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+  <conditionalFormatting sqref="G29 D29">
+    <cfRule type="cellIs" dxfId="31" priority="33" operator="equal">
       <formula>"NOT OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D26">
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
+  <conditionalFormatting sqref="D29">
+    <cfRule type="cellIs" dxfId="30" priority="31" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G16">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
+  <conditionalFormatting sqref="G18">
+    <cfRule type="cellIs" dxfId="29" priority="30" operator="equal">
       <formula>"NOT OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H16">
-    <cfRule type="cellIs" dxfId="13" priority="12" operator="equal">
+  <conditionalFormatting sqref="H18">
+    <cfRule type="cellIs" dxfId="28" priority="27" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",H16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="14" operator="containsText" text="yes">
-      <formula>NOT(ISERROR(SEARCH("yes",H16)))</formula>
+    <cfRule type="containsText" dxfId="27" priority="28" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="29" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",H18)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G27 D27">
+  <conditionalFormatting sqref="G30 D30">
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
+      <formula>"NOT OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30">
+    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
+      <formula>"ok"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6">
+    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",H6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6 D6">
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+      <formula>"NOT OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
+      <formula>"ok"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11">
+    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="19" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",H11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
+      <formula>"NOT OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23">
+    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",H23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G23 D23">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+      <formula>"NOT OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23">
     <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>"ok"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",H4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4 D4">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"NOT OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D27">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
-      <formula>"ok"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
-      <formula>"no"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",H5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="yes">
-      <formula>NOT(ISERROR(SEARCH("yes",H5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G5 D5">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
-      <formula>"NOT OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+  <conditionalFormatting sqref="D4">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",H9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="yes">
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="yes">
       <formula>NOT(ISERROR(SEARCH("yes",H9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G9">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+  <conditionalFormatting sqref="G9 D9">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"NOT OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>